<commit_message>
cambio en las listas y manejo de comentarios
</commit_message>
<xml_diff>
--- a/Casos de prueba.xlsx
+++ b/Casos de prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Curso Python\MisProyectosDjango\BibliotecaCircular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B217D7-F0F5-415C-B96F-CA9069B8C3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D7381C-888A-4FE7-9900-F3CAAE5E660C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2976" yWindow="2628" windowWidth="19104" windowHeight="9612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -80,13 +80,19 @@
   </si>
   <si>
     <t>Daniela Quaranta</t>
+  </si>
+  <si>
+    <t>Nuevo libro, revisar que aparerza en el listado. Modificar y luego verificar que que aparezcan los nuevos datos. Pruebo eliminar un libro</t>
+  </si>
+  <si>
+    <t>Boton buscar sin escribir nada o que no encuentre datos.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +115,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -158,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -181,6 +200,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,7 +425,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -486,12 +511,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="11"/>
       <c r="D7" s="8">
         <v>44651</v>
       </c>
@@ -518,11 +545,13 @@
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
     </row>
-    <row r="8" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8">
         <v>44651</v>

</xml_diff>